<commit_message>
Bổ sung báo cáo
</commit_message>
<xml_diff>
--- a/BaoCaoCacBai/Phân-công.xlsx
+++ b/BaoCaoCacBai/Phân-công.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9885"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Phân chia</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Đào Xuân Vương</t>
   </si>
   <si>
-    <t>Phạm Thu thảo</t>
-  </si>
-  <si>
     <t>Nguyễn Thị Cẩm Nhung</t>
   </si>
   <si>
@@ -86,13 +83,79 @@
   </si>
   <si>
     <t>Phạm Thanh Tùng và Hoàng T.T. Vân</t>
+  </si>
+  <si>
+    <t>Xây dựng phần mềm quản lý thư viện của Học viện Kỹ thuật Quân sự</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Xây dựng CSDL đầu sách, độc giả, thông tin mượn trả</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>Xây dựng module quản lý thông tin sách (thêm , sửa, xóa)</t>
+  </si>
+  <si>
+    <t>Xây dựng module quản lý thông tin đầu sách (Thêm, sửa, xóa)</t>
+  </si>
+  <si>
+    <t>Xây dựng module quản lý Thể loại (Thêm ,sửa ,xóa)</t>
+  </si>
+  <si>
+    <t>Xây dựng module quản lý Nhà xuất bản (Thêm ,sửa ,xóa)</t>
+  </si>
+  <si>
+    <t>Xây dựng module quản lý thông tin mượn trả_Phiếu mượn &amp; Chi tiết phiếu mượn (thêm, sửa, xóa)</t>
+  </si>
+  <si>
+    <t>Xây dựng module quản lý Lớp (Thêm ,sửa ,xóa)</t>
+  </si>
+  <si>
+    <t>Xây dựng module quản lý Người dùng (Thêm ,sửa ,xóa)</t>
+  </si>
+  <si>
+    <t>Phạm Thanh Tùng &amp; Đào Xuân Vương</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +186,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -132,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -155,13 +232,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -190,12 +279,65 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -462,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -524,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="3"/>
@@ -538,7 +680,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="3"/>
@@ -552,7 +694,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="3"/>
@@ -566,7 +708,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="3"/>
@@ -580,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="3"/>
@@ -594,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="3"/>
@@ -608,7 +750,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="3"/>
@@ -636,11 +778,190 @@
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" ht="63">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="47.25">
+      <c r="A14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" ht="94.5">
+      <c r="A15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="47.25">
+      <c r="A16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="47.25">
+      <c r="A17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="47.25">
+      <c r="A18" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="47.25">
+      <c r="A19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="31.5">
+      <c r="A20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="47.25">
+      <c r="A21" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="78.75">
+      <c r="A22" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="31.5">
+      <c r="A23" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="47.25">
+      <c r="A24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" ht="31.5">
+      <c r="A25" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="D26" s="13"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>